<commit_message>
feat: merged practice image gen with other images
</commit_message>
<xml_diff>
--- a/stimuli_hr/multipleye_stimuli_experiment_hr.xlsx
+++ b/stimuli_hr/multipleye_stimuli_experiment_hr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27016"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://erf-my.sharepoint.com/personal/skosutar_erf_hr/Documents/MultiplEYE CA21131/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{23C3B24B-E087-472E-8A7C-D790A388C7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B50598D0-76A7-4C27-8D69-837DF9362E1B}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{23C3B24B-E087-472E-8A7C-D790A388C7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DA95456-E1ED-4ADB-8696-50E83FCF73A0}"/>
   <bookViews>
     <workbookView xWindow="1230" yWindow="765" windowWidth="27570" windowHeight="14835" xr2:uid="{EF339F11-F4DE-4D0A-862E-E00578AF5D2A}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="237">
   <si>
     <t>stimulus_id</t>
   </si>
@@ -284,6 +284,42 @@
     <t>PopSci_MultiplEYE</t>
   </si>
   <si>
+    <t>Dobrodošli u MultiplEYE!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naziv „MultiplEYE“ igra je riječima “multilingualism” (engleski za višejezičnost) ili “multiple languages” (engleski za više jezika) te “eye” (engleski za oko) iz “eye-tracking” (engleski za praćenje pokreta oka). MultiplEYE je COST akcija koju financira Europska unija. COST akcije istraživačke su mreže koje podupire Europska suradnja u znanosti i tehnologiji ili skraćeno COST. Kao financijska organizacija COST podupire našu rastuću mrežu istraživača diljem Europe i šire osiguravajući financijsku pomoć za provođenje različitih aktivnosti umrežavanja. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Te aktivnosti uključuju sastanke radnih skupina, škole za dijeljenje vještina s mlađim istraživačima i znanstvene istraživačke posjete. Naziv projekta MultiplEYE COST Action je Omogućavanje prikupljanja višejezičnih podataka praćenjem pokreta oka u svrhu istraživanja ljudske i strojne obrade jezika. To znači da MultiplEYE COST Akcija ima za cilj poticati interdisciplinarnu mrežu istraživačkih skupina koje rade na prikupljanju podataka praćenjem pokreta oka tijekom čitanja u brojnim jezicima. </t>
+  </si>
+  <si>
+    <t>Cilj je podržati razvoj velikoga višejezičnog korpusa praćenja pokreta oka i omogućiti istraživačima da prikupe podatke dijeleći svoje znanje između različitih područja, uključujući lingvistiku, psihologiju, logopediju i računalnu znanost. To prikupljanje podataka može se zatim rabiti za proučavanje ljudske obrade jezika iz psiholingvističke perspektive kao i za poboljšavanje i procjenu računalne obrade jezika iz perspektive strojnog učenja.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Što je „praćenje pokreta oka“? Praćenje pokreta oka proces je mjerenja točke pogleda – gdje gledate – i pokreta očiju između fiksnih točaka pogleda. Uređaj za mjerenje položaja oka i pokreta oka naziva se uređaj za praćenje pokreta oka. Sastoji se od infracrvene kamere rabeći frekvenciju svjetlosti koja ne zamara oko niti ga ozljeđuje. </t>
+  </si>
+  <si>
+    <t>Uz pomoć algoritama za prepoznavanje slike, uređaj za praćenje pokreta oka može vrlo precizno procijeniti točke pogleda znajući položaj glave i očiju, udaljenost od zaslona u koji sudionik gleda i položaj uređaja. Praćenje pokreta oka korisna je tehnologija za mnoge primjene. Primjerice, može pomoći u otkrivanju umora tijekom vožnje ili može poduprijeti postupke probira i obuke u području medicine. Praćenje pokreta oka rabi se i u igricama, marketingu te interakciji čovjeka i računala.</t>
+  </si>
+  <si>
+    <t>Zašto je praćenje pokreta oka tijekom čitanja posebno zanimljivo za naš projekt? Dok čitate ove riječi, uređaj prati pokrete Vašeg oka kroz tekst. To pruža informaciju o tome koliko ste dugo gledali u tekst, ili točnije, koliko ste vremena proveli na svakoj riječi, koje ste riječi preskočili, na kojim ste se riječima zadržali i jeste li se morali vratiti i ponovno pročitati dijelove teksta da biste ga bolje razumjeli.</t>
+  </si>
+  <si>
+    <t>Dok Vaš mozak obrađuje sadržaj teksta, Vaši pokreti oka odražavaju velik dio jezične i kognitivne obrade koja se odvija gotovo u stvarnome vremenu. Stoga su snimljeni podatci zlatni rudnik informacija o tome kako povezujemo značenje teksta s gramatičkim strukturama. Oni pokazuju s kojim se dijelovima teksta mučimo, a koji su lako čitljivi. Na istraživačima je da kasnije objasne koji su jezični čimbenici uzrokovali određene vrste pokreta oka.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motivacija za Akcijom MultiplEYE je ta da su podatci o praćenju pokreta oka još uvijek nedostatni, posebice u manjim jezicima. Ovako opsežno prikupljanje podataka izazov je u smislu razvoja i dogovora o eksperimentalnom dizajnu, složenosti i vrstama tekstova koje će sudionici čitati. Ostale odluke koje se čine manje važnima, ali su zapravo itekako bitne, uključuju vrstu i veličinu fonta kojim je tekst napisan, redoslijed tekstova, eksperimentalni postupak i način obrade podataka. </t>
+  </si>
+  <si>
+    <t>No jednom kada bude prikupljen, ovaj skup podataka omogućit će nam da istražimo mnoge teme u okviru psiholingvistike i računalne lingvistike. Na primjer, moći ćemo usporediti čitanje u različitim jezicima. Utječe li vrsta pisma, primjerice latinica naspram ćirilice ili arapskog pisma, na vrijeme čitanja? U području računalne obrade teksta, podatci praćenja pokreta oka mogli bi se upotrijebiti za unaprjeđenje umjetne inteligencije koja oponaša ljudski proces čitanja. To bi se moglo upotrijebiti za izgradnju boljih sustava strojnog prevođenja ili za poboljšanje automatskog izdvajanja ključnih riječi iz teksta.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prikupljanje podataka o praćenju pokreta oka mnogih sudionika, uključujući i Vas, tijekom čitanja tekstova u različitim jezicima, bit će izvrstan temelj za naše istraživanje. To će biti glavni čimbenik koji će omogućiti da naša istraživačka mreža postane uspješan pothvat. Nadamo se kako ćemo, podupiranjem i povezivanjem velike skupine istraživača, utrti put unaprjeđenju istraživanja u različitim područjima lingvistike. </t>
+  </si>
+  <si>
+    <t>Glavni rezultati Akcije MultiplEYE bit će veliki skup podataka praćenja pokreta oka u brojnim jezicima i platforma za nove suradnje koje će se oslanjati na tu vrstu podataka. Čitanjem ovoga teksta već podržavate naš cilj dopuštajući nam da prikupimo i analiziramo Vaše pokrete oka tijekom čitanja i razumijevanja jezika. Hvala Vam!</t>
+  </si>
+  <si>
     <t>multiple choice</t>
   </si>
   <si>
@@ -344,97 +380,34 @@
     <t>Ins_HumanRights</t>
   </si>
   <si>
+    <t>Opća deklaracija o ljudskim pravima - preambula</t>
+  </si>
+  <si>
+    <t>Budući da je priznanje urođenog dostojanstva te jednakih i neotuđivih prava svih članova ljudske obitelji temelj slobode, pravde i mira u svijetu,</t>
+  </si>
+  <si>
+    <t>budući da je nepoštivanje i zanemarivanje ljudskih prava rezultiralo barbarskim postupcima koji vrijeđaju savjest čovječanstva i da je izgradnja svijeta u kojemu će ljudska bića uživati slobodu govora i uvjerenja te biti slobodna od straha i neimaštine, proglašena najvećom težnjom svih ljudi,</t>
+  </si>
+  <si>
+    <t>budući da je bitno ljudska prava zaštititi vladavinom prava, kako čovjek ne bi morao pribjeći, kao krajnjem sredstvu, pobuni protiv tiranije i ugnjetavanja,</t>
+  </si>
+  <si>
+    <t>budući da je bitno promicati razvoj prijateljskih odnosa među narodima,</t>
+  </si>
+  <si>
+    <t>budući da su narodi Ujedinjenih naroda u Povelji ponovno potvrdili svoju vjeru u temeljna ljudska prava, u dostojanstvo i vrijednost ljudske osobe i jednaka prava muškaraca i žena te odlučili promicati društveni napredak i bolje uvjete života u većoj slobodi,</t>
+  </si>
+  <si>
+    <t>budući da su se države članice obvezale da u suradnji s Ujedinjenim narodima osiguraju promicanje općeg poštovanja i primjene ljudskih prava i temeljnih sloboda,</t>
+  </si>
+  <si>
+    <t>budući da je opće razumijevanje tih prava i sloboda od najvećeg značaja za puno ostvarenje te obveze,</t>
+  </si>
+  <si>
+    <t>sada, stoga, Opća skupština proglašava ovu Opću deklaraciju o ljudskim pravima kao zajedničko mjerilo postignuća svih naroda i nacija, kako bi svaki pojedinac i svako tijelo u društvu, imajući ovu Deklaraciju stalno na umu, težili poučavanjem i obrazovanjem promicati poštovanje ovih ljudskih prava i sloboda te kako bi se postupnim domaćim i međunarodnim mjerama osiguralo njihovo opće i djelotvorno priznanje i primjena među narodima država članica i među narodima na područjima pod njihovom jurisdikcijom.</t>
+  </si>
+  <si>
     <t>Ins_EURLex</t>
-  </si>
-  <si>
-    <t>Lit_Alchemist</t>
-  </si>
-  <si>
-    <t>Lit_Emperor_Clothes</t>
-  </si>
-  <si>
-    <t>Lit_Harry_Potter</t>
-  </si>
-  <si>
-    <t>Lit_MagicMountain</t>
-  </si>
-  <si>
-    <t>Lit_NorthWind</t>
-  </si>
-  <si>
-    <t>Lit_Solaris</t>
-  </si>
-  <si>
-    <t>Lit_BrokenApril</t>
-  </si>
-  <si>
-    <t>Arg_PisaRapaNui</t>
-  </si>
-  <si>
-    <t>Arg_PisaCowsMilk</t>
-  </si>
-  <si>
-    <t>Dobrodošli u MultiplEYE!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naziv „MultiplEYE“ igra je riječima “multilingualism” (engleski za višejezičnost) ili “multiple languages” (engleski za više jezika) te “eye” (engleski za oko) iz “eye-tracking” (engleski za praćenje pokreta oka). MultiplEYE je COST akcija koju financira Europska unija. COST akcije istraživačke su mreže koje podupire Europska suradnja u znanosti i tehnologiji ili skraćeno COST. Kao financijska organizacija COST podupire našu rastuću mrežu istraživača diljem Europe i šire osiguravajući financijsku pomoć za provođenje različitih aktivnosti umrežavanja. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Te aktivnosti uključuju sastanke radnih skupina, škole za dijeljenje vještina s mlađim istraživačima i znanstvene istraživačke posjete. Naziv projekta MultiplEYE COST Action je Omogućavanje prikupljanja višejezičnih podataka praćenjem pokreta oka u svrhu istraživanja ljudske i strojne obrade jezika. To znači da MultiplEYE COST Akcija ima za cilj poticati interdisciplinarnu mrežu istraživačkih skupina koje rade na prikupljanju podataka praćenjem pokreta oka tijekom čitanja u brojnim jezicima. </t>
-  </si>
-  <si>
-    <t>Cilj je podržati razvoj velikoga višejezičnog korpusa praćenja pokreta oka i omogućiti istraživačima da prikupe podatke dijeleći svoje znanje između različitih područja, uključujući lingvistiku, psihologiju, logopediju i računalnu znanost. To prikupljanje podataka može se zatim rabiti za proučavanje ljudske obrade jezika iz psiholingvističke perspektive kao i za poboljšavanje i procjenu računalne obrade jezika iz perspektive strojnog učenja.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Što je „praćenje pokreta oka“? Praćenje pokreta oka proces je mjerenja točke pogleda – gdje gledate – i pokreta očiju između fiksnih točaka pogleda. Uređaj za mjerenje položaja oka i pokreta oka naziva se uređaj za praćenje pokreta oka. Sastoji se od infracrvene kamere rabeći frekvenciju svjetlosti koja ne zamara oko niti ga ozljeđuje. </t>
-  </si>
-  <si>
-    <t>Uz pomoć algoritama za prepoznavanje slike, uređaj za praćenje pokreta oka može vrlo precizno procijeniti točke pogleda znajući položaj glave i očiju, udaljenost od zaslona u koji sudionik gleda i položaj uređaja. Praćenje pokreta oka korisna je tehnologija za mnoge primjene. Primjerice, može pomoći u otkrivanju umora tijekom vožnje ili može poduprijeti postupke probira i obuke u području medicine. Praćenje pokreta oka rabi se i u igricama, marketingu te interakciji čovjeka i računala.</t>
-  </si>
-  <si>
-    <t>Zašto je praćenje pokreta oka tijekom čitanja posebno zanimljivo za naš projekt? Dok čitate ove riječi, uređaj prati pokrete Vašeg oka kroz tekst. To pruža informaciju o tome koliko ste dugo gledali u tekst, ili točnije, koliko ste vremena proveli na svakoj riječi, koje ste riječi preskočili, na kojim ste se riječima zadržali i jeste li se morali vratiti i ponovno pročitati dijelove teksta da biste ga bolje razumjeli.</t>
-  </si>
-  <si>
-    <t>Dok Vaš mozak obrađuje sadržaj teksta, Vaši pokreti oka odražavaju velik dio jezične i kognitivne obrade koja se odvija gotovo u stvarnome vremenu. Stoga su snimljeni podatci zlatni rudnik informacija o tome kako povezujemo značenje teksta s gramatičkim strukturama. Oni pokazuju s kojim se dijelovima teksta mučimo, a koji su lako čitljivi. Na istraživačima je da kasnije objasne koji su jezični čimbenici uzrokovali određene vrste pokreta oka.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motivacija za Akcijom MultiplEYE je ta da su podatci o praćenju pokreta oka još uvijek nedostatni, posebice u manjim jezicima. Ovako opsežno prikupljanje podataka izazov je u smislu razvoja i dogovora o eksperimentalnom dizajnu, složenosti i vrstama tekstova koje će sudionici čitati. Ostale odluke koje se čine manje važnima, ali su zapravo itekako bitne, uključuju vrstu i veličinu fonta kojim je tekst napisan, redoslijed tekstova, eksperimentalni postupak i način obrade podataka. </t>
-  </si>
-  <si>
-    <t>No jednom kada bude prikupljen, ovaj skup podataka omogućit će nam da istražimo mnoge teme u okviru psiholingvistike i računalne lingvistike. Na primjer, moći ćemo usporediti čitanje u različitim jezicima. Utječe li vrsta pisma, primjerice latinica naspram ćirilice ili arapskog pisma, na vrijeme čitanja? U području računalne obrade teksta, podatci praćenja pokreta oka mogli bi se upotrijebiti za unaprjeđenje umjetne inteligencije koja oponaša ljudski proces čitanja. To bi se moglo upotrijebiti za izgradnju boljih sustava strojnog prevođenja ili za poboljšanje automatskog izdvajanja ključnih riječi iz teksta.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prikupljanje podataka o praćenju pokreta oka mnogih sudionika, uključujući i Vas, tijekom čitanja tekstova u različitim jezicima, bit će izvrstan temelj za naše istraživanje. To će biti glavni čimbenik koji će omogućiti da naša istraživačka mreža postane uspješan pothvat. Nadamo se kako ćemo, podupiranjem i povezivanjem velike skupine istraživača, utrti put unaprjeđenju istraživanja u različitim područjima lingvistike. </t>
-  </si>
-  <si>
-    <t>Glavni rezultati Akcije MultiplEYE bit će veliki skup podataka praćenja pokreta oka u brojnim jezicima i platforma za nove suradnje koje će se oslanjati na tu vrstu podataka. Čitanjem ovoga teksta već podržavate naš cilj dopuštajući nam da prikupimo i analiziramo Vaše pokrete oka tijekom čitanja i razumijevanja jezika. Hvala Vam!</t>
-  </si>
-  <si>
-    <t>Opća deklaracija o ljudskim pravima - preambula</t>
-  </si>
-  <si>
-    <t>Budući da je priznanje urođenog dostojanstva te jednakih i neotuđivih prava svih članova ljudske obitelji temelj slobode, pravde i mira u svijetu,</t>
-  </si>
-  <si>
-    <t>budući da je nepoštivanje i zanemarivanje ljudskih prava rezultiralo barbarskim postupcima koji vrijeđaju savjest čovječanstva i da je izgradnja svijeta u kojemu će ljudska bića uživati slobodu govora i uvjerenja te biti slobodna od straha i neimaštine, proglašena najvećom težnjom svih ljudi,</t>
-  </si>
-  <si>
-    <t>budući da je bitno ljudska prava zaštititi vladavinom prava, kako čovjek ne bi morao pribjeći, kao krajnjem sredstvu, pobuni protiv tiranije i ugnjetavanja,</t>
-  </si>
-  <si>
-    <t>budući da je bitno promicati razvoj prijateljskih odnosa među narodima,</t>
-  </si>
-  <si>
-    <t>budući da su narodi Ujedinjenih naroda u Povelji ponovno potvrdili svoju vjeru u temeljna ljudska prava, u dostojanstvo i vrijednost ljudske osobe i jednaka prava muškaraca i žena te odlučili promicati društveni napredak i bolje uvjete života u većoj slobodi,</t>
-  </si>
-  <si>
-    <t>budući da su se države članice obvezale da u suradnji s Ujedinjenim narodima osiguraju promicanje općeg poštovanja i primjene ljudskih prava i temeljnih sloboda,</t>
-  </si>
-  <si>
-    <t>budući da je opće razumijevanje tih prava i sloboda od najvećeg značaja za puno ostvarenje te obveze,</t>
-  </si>
-  <si>
-    <t>sada, stoga, Opća skupština proglašava ovu Opću deklaraciju o ljudskim pravima kao zajedničko mjerilo postignuća svih naroda i nacija, kako bi svaki pojedinac i svako tijelo u društvu, imajući ovu Deklaraciju stalno na umu, težili poučavanjem i obrazovanjem promicati poštovanje ovih ljudskih prava i sloboda te kako bi se postupnim domaćim i međunarodnim mjerama osiguralo njihovo opće i djelotvorno priznanje i primjena među narodima država članica i među narodima na područjima pod njihovom jurisdikcijom.</t>
   </si>
   <si>
     <t>IZVJEŠĆE KOMISIJE VIJEĆU Izvješće o napretku pokazatelja za mobilnost u svrhu učenja</t>
@@ -466,6 +439,9 @@
     <t>Referentnom vrijednosti EU-a mjeri se broj osoba s diplomom koje su bile mobilne tijekom studija i uspješno su stekle svoje kvalifikacije. Njome se izravno ne određuje zemljopisno područje, ali se u Zaključcima iz 2011. ističe da se „mobilnost u svrhu učenja definira kao fizička mobilnost te u obzir uzima mobilnost diljem svijeta”. Mjerenje pokazatelja referentne vrijednosti za mobilnost u početnome strukovnom obrazovanju i osposobljavanju u praksi je ograničeno instrumentom koji je izrijekom naveden u Zaključcima (anketa kućanstava koja se provodi na određenoj velikoj dobnoj skupini), dok izvor za pokazatelj referentne vrijednosti za visoko obrazovanje nije naveden.</t>
   </si>
   <si>
+    <t>Lit_Alchemist</t>
+  </si>
+  <si>
     <t>Alkemičar - 1. poglavlje</t>
   </si>
   <si>
@@ -481,30 +457,10 @@
     <t>– Toliko su se već navikle na mene da poznaju moju satnicu – reče tihim glasom. Zamisli se na trenutak i pomisli kako bi moglo biti i obrnuto: da se on navikao na satnicu svojih ovaca. Bilo je pak ovaca kojima je duže trebalo da ustanu. Mladić je budio jednu po jednu svojim štapom, zovući svaku njenim imenom. Oduvijek je vjerovao da su ovce u stanju razumjeti ono što im je govorio.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Stoga im je ponekad čitao ulomke iz knjiga koje su ga dojmile, ili govorio o samoći i o radostima pastira u polju,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ili se osvrtao na posljednje novosti što ih je vidio u gradovima kojima je običavao prolaziti. No, u posljednja dva dana njegova je tema bila isključivo jedna: djevojka, trgovčeva kćer, koja je živjela u gradu u koji će stići za četiri dana. Bio je tamo samo jedanput prošle godine. Trgovac je bio vlasnik dućana s tkaninama i uvijek je volio gledati kako se ovce strižu pred njim, da ne bi bilo nikakve prijevare. Neki ga je prijatelj bio uputio u dućan, i tamo je pastir poveo svoje ovce.  </t>
-    </r>
-  </si>
-  <si>
-    <t>comment: the red part is one sentence in Croatian, and two sentences in English. And the second sentence is in the next screen. This is why we transferred the entire big sentence to the new screen in Croatian</t>
+    <t xml:space="preserve">Stoga im je ponekad čitao ulomke iz knjiga koje su ga dojmile, ili govorio o samoći i o radostima pastira u polju, ili se osvrtao na posljednje novosti što ih je vidio u gradovima kojima je običavao prolaziti. No, u posljednja dva dana njegova je tema bila isključivo jedna: djevojka, trgovčeva kćer, koja je živjela u gradu u koji će stići za četiri dana. Bio je tamo samo jedanput prošle godine. Trgovac je bio vlasnik dućana s tkaninama i uvijek je volio gledati kako se ovce strižu pred njim, da ne bi bilo nikakve prijevare. Neki ga je prijatelj bio uputio u dućan, i tamo je pastir poveo svoje ovce.  </t>
+  </si>
+  <si>
+    <t>Lit_Emperor_Clothes</t>
   </si>
   <si>
     <t>Carevo novo ruho</t>
@@ -585,6 +541,9 @@
     <t>Dosad nijedna careva odjeća nije doživjela takvo priznanje. Ali najednom je neko dijete povikalo: – Pa car je gol! – Ah, bože moj, taj nedužni glasić! – zabrzao je uplašeni otac. Ali već istog trenutka se začuo šapat: – Dijete kaže da je car gol! Car je bez odore! I odmah zatim počeše vikati svi u jedan glas: – Car je bez odore! Bez odore! Car je pretrnuo – vidio je i sam da je bez odore, ali je ipak odlučio ostati do kraja u procesiji pa je zauzeo još dostojanstvenije držanje. A komornici iza njega i dalje su nosili nepostojeće skute.</t>
   </si>
   <si>
+    <t>Lit_Harry_Potter</t>
+  </si>
+  <si>
     <t>Harry Potter i Kamen Mudraca. 1. poglavlje: Dječak koji je ostao živ</t>
   </si>
   <si>
@@ -606,6 +565,9 @@
     <t>Nitko od njih nije primijetio veliku žutosmeđu sovu kako je proletjela pokraj njihovih prozora. U osam i pol gospodin Dursley uzeo je svoju torbu, letimice cjelunuo gospođu Dursley u obraz i pokušao na rastanku poljubiti i Dudleyja, ali ga je promašio jer je Dudleyja upravo spopao bijes pa je kašicu bacao oko sebe po zidovima. "Vražji malac!" propenta gospodin Dursley izlazeći iz kuće. Sjeo je u svoja kola i izašao natraške na Kalinin prilaz ispred broja četiri.</t>
   </si>
   <si>
+    <t>Lit_MagicMountain</t>
+  </si>
+  <si>
     <t xml:space="preserve">Čarobna gora - Nakana </t>
   </si>
   <si>
@@ -624,12 +586,18 @@
     <t>Stoga pripovjedač neće ispripovjediti priču o Hansu dok bi dlanom o dlan. Neće mu dostajati sedam dana jednog tjedna, pa čak ni sedam mjeseci. Najbolje će biti da se ne pitamo koliko će zemaljskog vremena proteći dok je ne dotjera do kraja. Valjda neće, za ime Božje, biti baš sedam godina! A sad, počnimo!</t>
   </si>
   <si>
+    <t>Lit_NorthWind</t>
+  </si>
+  <si>
     <t>Sjeverni vjetar i sunce</t>
   </si>
   <si>
     <t>Sjeverni vjetar i sunce su raspravljali o tome tko je od njih dvoje jači, kad je naišao putnik umotan u topli kaput. Dogovorili su se da će onaj koji prvi putnika natjera da skine kaput biti proglašen  jačim. U tom trenutku, sjeverni vjetar je zapuhao što je jače mogao, ali što je više puhao, putnik se sve više umotavao u svoj kaput. Stoga je na kraju sjeverni vjetar odustao! Tada je sunce počelo sjati i putnik je odmah skinuo svoj kaput. Sjeverni vjetar je tada bio primoran priznati, da je Sunce jače od njega.</t>
   </si>
   <si>
+    <t>Lit_Solaris</t>
+  </si>
+  <si>
     <t>Solaris - 2. poglavlje: Solaristi</t>
   </si>
   <si>
@@ -639,30 +607,7 @@
     <t>Naizmjenične perturbacije sužavaju i rastežu orbitu planeta i zameci života, ako nastanu, podliježu uništenju od užarenih zraka ili ledene hladnoće. Te se promjene događaju u razdoblju milijuna godina, dakle - u astronomskim ili biološkim razmjerima (jer evolucija traži stotine milijuna, ako ne milijardi godina) u vrlo kratkome vremenu.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Solaris se prema prvotnim istraživanjima trebao tijekom </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>petsto tisuća</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> godina približiti svojemu crvenom suncu na razdaljinu od polovine astronomske jedinice, a nakon daljnjega milijuna - pasti u njegov užareni bezdan. Ali već nakon dvadesetak godina došlo se do uvjerenja da njegova putanja uopće ne najavljuje očekivane promjene, kao da je bila posve postojana, onako stalna kao što su to putanje planeta našega Sunčeva sustava.</t>
-    </r>
+    <t>Solaris se prema prvotnim istraživanjima trebao tijekom petsto tisuća godina približiti svojemu crvenom suncu na razdaljinu od polovine astronomske jedinice, a nakon daljnjega milijuna - pasti u njegov užareni bezdan. Ali već nakon dvadesetak godina došlo se do uvjerenja da njegova putanja uopće ne najavljuje očekivane promjene, kao da je bila posve postojana, onako stalna kao što su to putanje planeta našega Sunčeva sustava.</t>
   </si>
   <si>
     <t>Promatranja su, sada s najvećom točnošću, ponovljena i izračuni su potvrdili ono što je već bilo poznato: Solaris ima nestalnu orbitu. Od jednoga između nekoliko stotina planeta, koliko ih se godišnje otkriva, a koje kratkim zabilješkama s elementima njihova kretanja bivaju ubačene u velike statistike, Solaris je tada napredovao u rang tijela dostojnog posebne pozornosti.</t>
@@ -701,20 +646,7 @@
     <t>U inat tom konzervativizmu, nastajale su hipoteze koje su zvučale poput jedne od bolje obrađenih Civita-Vitti, da je ocean rezultat dijalektičkog razvitka: od svojega prvobitnog oblika, od praoceana, rastvora lijeno reaktivnih kemijskih tijela, uspio pod pritiskom uvjeta (to znači promjena orbite koje su ugrožavale njegovu opstojnost), bez posredovanja svih zemaljskih razvojnih stupnjeva, zaobilazeći dakle nastanak jednostaničnih i višestaničnih oblika, biljnu i životinjsku evoluciju, bez razvoja živčanoga sustava, mozga, smjesta preskočiti u stadij homeostatičnog oceana.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Drugačije rečeno, nije se poput zemaljskih organizama tijekom stotina milijuna godina prilagođavao okolišu, da bi tek nakon golemog vremena dao začetak razumne rase, već je nad svojim okolišem zavladao odmah. Bilo je to vrlo originalno, samo što i nadalje nitko nije znao kako sirupasta hladetina može stabilizirati orbitu nebeskog tijela. Već zamalo stoljeće, bili su poznati uređaji koji su stvarali umjetna polja sila i gravitacije - gravitori </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ali nitko si nije mogao čak ni zamisliti kako takav rezultat, koji u gravitorima nastaje kao proizvod složenih nuklearnih reakcija i strahovitih temperatura, može postići bezoblična smola. ------&gt; COMMENT - red part is a completely new sentence in ENG and therefore in the next screen. </t>
-    </r>
+    <t xml:space="preserve">Drugačije rečeno, nije se poput zemaljskih organizama tijekom stotina milijuna godina prilagođavao okolišu, da bi tek nakon golemog vremena dao začetak razumne rase, već je nad svojim okolišem zavladao odmah. Bilo je to vrlo originalno, samo što i nadalje nitko nije znao kako sirupasta hladetina može stabilizirati orbitu nebeskog tijela. Već zamalo stoljeće, bili su poznati uređaji koji su stvarali umjetna polja sila i gravitacije - gravitori ali nitko si nije mogao čak ni zamisliti kako takav rezultat, koji u gravitorima nastaje kao proizvod složenih nuklearnih reakcija i strahovitih temperatura, može postići bezoblična smola. </t>
   </si>
   <si>
     <t>U novinama, koje su u to doba radi poticanja zanimanja čitatelja i na užas znanstvenika bile prepune izmišljotina na temu Solarisove tajne, nije manjkalo ni takvih tvrdnji da je planetarni ocean... daleki rođak zemaljskih električnih jegulja. Kada se problem, barem u stanovitoj mjeri, uspjelo riješiti, pokazalo se da je objašnjenje, kako se to često i kasnije događalo sa Solarisom, na mjesto jedne zagonetke podmetnulo drugu, možda još začudniju.</t>
@@ -724,6 +656,9 @@
   </si>
   <si>
     <t>Kada je to izrečeno, u znanstvenome svijetu je izbila jedna od najsilovitijih oluja našeg stoljeća. Najpoštovanije, općepriznate teorije, rušile su se u prah, u znanstvenoj literaturi pojavljivali su se najheretičniji članci, dok je alternativa genijalni ocean ili gravitacijska hladetina raspalila sve umove.</t>
+  </si>
+  <si>
+    <t>Lit_BrokenApril</t>
   </si>
   <si>
     <t>Slomljeni travanj - 3. poglavlje</t>
@@ -763,6 +698,9 @@
     <t>S druge strane, bilo je drugih – bili su malobrojni – koji su se prilično zabavljali slušajući sva ta mišljenja, kao da žele reći: „Dobro, idi gore na sjever među planinske nimfe. Dobro će doći oboma, a posebno Bessianu.“</t>
   </si>
   <si>
+    <t>Arg_PisaRapaNui</t>
+  </si>
+  <si>
     <t>Uskršnji otok</t>
   </si>
   <si>
@@ -816,6 +754,9 @@
     <t>Pouka ove čudesne ali zastrašujuće knjige jest da su ljudi u prošlosti odlučili uništiti svoj okoliš sječom svih stabala i lovom na životinjske vrste sve do njihova istrebljenja. Autor optimistično napominje da mi možemo odlučiti ne ponoviti iste greške danas. Ova dobro napisana knjiga zaslužuje pažnju svih koji brinu za okoliš.</t>
   </si>
   <si>
+    <t>Arg_PisaCowsMilk</t>
+  </si>
+  <si>
     <t>Kravlje mlijeko</t>
   </si>
   <si>
@@ -843,8 +784,8 @@
 Međunarodno udruženje za mliječne proizvode, 27. rujna 2007.</t>
   </si>
   <si>
-    <t>Anna, Christopher and Sam are talking about the decision of the coffee shop owner to stop selling cow’s milk. Sam says, “Maybe cow’s milk is becoming too expensive.” Christopher is looking at his smartphone. “Maybe, but I did a web search on cow’s milk too. I’m going to text you the link to a more recent article that may explain it.”
-Anna and Sam open the link Christopher sent and read the article, “Just Say ‘No’ to Cow’s Milk!”  -------------------&gt; comment - for some reason this part is completely missing in the CRO version</t>
+    <t>Anna, Christopher i Sam razgovaraju o odluci vlasnika zdravljaka da prestaje prodavati kravlje mlijeko. Sam kaže: "Možda je kravlje mlijeko postalo preskupo." Christopher gleda u svoj pametni telefon. “Možda je tako, ali i ja sam potražio informacije o kravljem mlijeku na internetu. Poslat ću vam poruku s poveznicom na nedavni članak koji bi to mogao objasniti.”
+Anna i Sam otvaraju poveznicu koju im je Christopher poslao i čitaju članak: "Recite 'ne' kravljem mlijeku!</t>
   </si>
   <si>
     <t>www.zdravljedanas.hr/mlijeko
@@ -872,7 +813,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -908,6 +849,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -916,12 +858,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1030,19 +969,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperveza" xfId="1" builtinId="8"/>
-    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="66">
     <dxf>
@@ -1494,7 +1433,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1792,11 +1731,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9016B68B-E770-4A04-A8EB-C009482E3DEC}">
   <dimension ref="A1:BY29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AK1" sqref="AK1"/>
+    <sheetView tabSelected="1" topLeftCell="Q9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
@@ -1823,7 +1762,7 @@
     <col min="78" max="78" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77" ht="30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2056,7 +1995,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:77" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:77" ht="120">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2064,1722 +2003,1720 @@
         <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>92</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>92</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>106</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM2" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>92</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>93</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>94</v>
-      </c>
-      <c r="BL2" t="s">
+      <c r="BP2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BM2" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP2" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="BQ2" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="BR2" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BU2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BV2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BW2" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:77" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:77" ht="105">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="AK3" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="AV3" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="AW3" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="AX3" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="AY3" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AZ3" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BA3" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BB3" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="BC3" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BD3" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="BK3" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="BL3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP3" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BM3" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP3" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="BQ3" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="BR3" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BU3" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BV3" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BW3" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:77" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77" ht="165">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="AL4" s="1" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="AV4" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="AW4" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="AX4" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="AY4" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AZ4" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BA4" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BB4" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="BC4" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BD4" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="BK4" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="BL4" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP4" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BM4" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP4" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="BQ4" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="BR4" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BU4" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BV4" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BW4" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:77" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:77" ht="106.5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="W5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL5" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG5" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL5" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="AM5" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="AV5" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="AW5" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="AX5" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="AY5" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AZ5" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BA5" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BB5" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="BC5" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BD5" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="BK5" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="BL5" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM5" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP5" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BM5" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP5" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="BQ5" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="BR5" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BU5" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BV5" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BW5" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:77" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77" ht="120">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK6" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL6" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM6" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="AN6" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="AO6" s="1" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="AV6" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="AW6" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="AX6" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="AY6" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AZ6" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BA6" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BB6" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="BC6" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BD6" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="BK6" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="BL6" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM6" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP6" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BM6" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP6" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="BQ6" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="BR6" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BU6" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BV6" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BW6" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:77" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77" ht="90">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG7" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH7" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ7" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL7" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN7" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="AO7" s="1" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="AV7" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="AW7" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="AX7" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="AY7" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AZ7" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BA7" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BB7" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="BC7" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BD7" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="BK7" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="BL7" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM7" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP7" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BM7" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP7" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="BQ7" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="BR7" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BU7" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BV7" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BW7" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:77" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77" ht="105">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO8" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD8" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI8" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ8" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK8" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO8" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="AV8" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="AW8" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="AX8" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="AY8" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AZ8" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BA8" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BB8" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="BC8" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BD8" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="BK8" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="BL8" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM8" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP8" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BM8" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP8" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="BQ8" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="BR8" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BU8" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BV8" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BW8" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:77" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77" ht="90">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AV9" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK9" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL9" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM9" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN9" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO9" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AV9" t="s">
-        <v>91</v>
-      </c>
       <c r="AW9" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="AX9" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="AY9" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AZ9" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BA9" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BB9" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="BC9" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BD9" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="BK9" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="BL9" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM9" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP9" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BM9" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP9" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="BQ9" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="BR9" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BU9" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BV9" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BW9" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:77" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77" ht="106.5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>103</v>
+      </c>
+      <c r="AW10" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="U10" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ10" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK10" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM10" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN10" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO10" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AV10" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW10" t="s">
-        <v>92</v>
-      </c>
       <c r="AX10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="AY10" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AZ10" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BA10" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BB10" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="BC10" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BD10" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="BK10" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="BL10" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM10" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BM10" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP10" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="BQ10" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="BR10" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BU10" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BV10" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BW10" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:77" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77" ht="90">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>103</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>104</v>
+      </c>
+      <c r="AX11" t="s">
         <v>105</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD11" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG11" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL11" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN11" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AV11" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>92</v>
-      </c>
-      <c r="AX11" t="s">
-        <v>93</v>
-      </c>
       <c r="AY11" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AZ11" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BA11" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BB11" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="BC11" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BD11" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="BK11" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="BL11" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM11" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BM11" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP11" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="BQ11" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="BR11" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BU11" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BV11" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BW11" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:77" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:77" ht="120">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AV12" t="s">
+        <v>103</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>104</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>105</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>92</v>
+      </c>
+      <c r="BA12" t="s">
+        <v>92</v>
+      </c>
+      <c r="BB12" t="s">
+        <v>103</v>
+      </c>
+      <c r="BC12" t="s">
+        <v>104</v>
+      </c>
+      <c r="BD12" t="s">
+        <v>105</v>
+      </c>
+      <c r="BK12" t="s">
         <v>106</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y12" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK12" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN12" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AV12" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW12" t="s">
-        <v>92</v>
-      </c>
-      <c r="AX12" t="s">
-        <v>93</v>
-      </c>
-      <c r="AY12" t="s">
-        <v>80</v>
-      </c>
-      <c r="AZ12" t="s">
-        <v>80</v>
-      </c>
-      <c r="BA12" t="s">
-        <v>80</v>
-      </c>
-      <c r="BB12" t="s">
-        <v>91</v>
-      </c>
-      <c r="BC12" t="s">
-        <v>92</v>
-      </c>
-      <c r="BD12" t="s">
-        <v>93</v>
-      </c>
-      <c r="BK12" t="s">
-        <v>94</v>
-      </c>
       <c r="BL12" t="s">
+        <v>107</v>
+      </c>
+      <c r="BM12" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP12" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BM12" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP12" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="BQ12" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="BR12" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BU12" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BV12" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BW12" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:77" ht="150" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:77" ht="137.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>103</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>104</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>105</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>92</v>
+      </c>
+      <c r="BA13" t="s">
+        <v>92</v>
+      </c>
+      <c r="BB13" t="s">
+        <v>103</v>
+      </c>
+      <c r="BC13" t="s">
+        <v>104</v>
+      </c>
+      <c r="BD13" t="s">
+        <v>105</v>
+      </c>
+      <c r="BK13" t="s">
+        <v>106</v>
+      </c>
+      <c r="BL13" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="J13" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="K13" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG13" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH13" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI13" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK13" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL13" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AN13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AV13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW13" t="s">
-        <v>92</v>
-      </c>
-      <c r="AX13" t="s">
-        <v>93</v>
-      </c>
-      <c r="AY13" t="s">
-        <v>80</v>
-      </c>
-      <c r="AZ13" t="s">
-        <v>80</v>
-      </c>
-      <c r="BA13" t="s">
-        <v>80</v>
-      </c>
-      <c r="BB13" t="s">
-        <v>91</v>
-      </c>
-      <c r="BC13" t="s">
-        <v>92</v>
-      </c>
-      <c r="BD13" t="s">
-        <v>93</v>
-      </c>
-      <c r="BK13" t="s">
-        <v>94</v>
-      </c>
-      <c r="BL13" t="s">
+      <c r="BM13" t="s">
+        <v>108</v>
+      </c>
+      <c r="BP13" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="BM13" t="s">
-        <v>96</v>
-      </c>
-      <c r="BP13" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="BQ13" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="BR13" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="BU13" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="BV13" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="BW13" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:77">
       <c r="H15" s="5"/>
     </row>
-    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:18">
       <c r="M17" s="2"/>
       <c r="R17" s="2"/>
     </row>
-    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:18">
       <c r="E19" s="2"/>
       <c r="M19" s="2"/>
       <c r="R19" s="2"/>
     </row>
-    <row r="20" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:18">
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:18">
       <c r="E21" s="2"/>
       <c r="H21" s="2"/>
       <c r="M21" s="2"/>
       <c r="R21" s="2"/>
     </row>
-    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:18">
       <c r="D22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:18">
       <c r="E23" s="2"/>
       <c r="H23" s="2"/>
       <c r="M23" s="2"/>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:18">
       <c r="D24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:18">
       <c r="E25" s="2"/>
       <c r="H25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:18">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:18">
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:18">
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:18">
       <c r="H29" s="2"/>
     </row>
   </sheetData>
@@ -3802,12 +3739,12 @@
   <dimension ref="A1:BY14"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O3" sqref="A1:XFD1048576"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77">
       <c r="A1" s="8"/>
       <c r="B1" s="9"/>
       <c r="C1" s="10"/>
@@ -3886,7 +3823,7 @@
       <c r="BX1" s="9"/>
       <c r="BY1" s="11"/>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:77">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="5"/>
@@ -3965,7 +3902,7 @@
       <c r="BX2" s="7"/>
       <c r="BY2" s="12"/>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:77">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="10"/>
@@ -4044,7 +3981,7 @@
       <c r="BX3" s="9"/>
       <c r="BY3" s="11"/>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -4123,7 +4060,7 @@
       <c r="BX4" s="7"/>
       <c r="BY4" s="12"/>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:77">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
@@ -4202,7 +4139,7 @@
       <c r="BX5" s="9"/>
       <c r="BY5" s="11"/>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="5"/>
@@ -4281,7 +4218,7 @@
       <c r="BX6" s="7"/>
       <c r="BY6" s="12"/>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
@@ -4360,7 +4297,7 @@
       <c r="BX7" s="9"/>
       <c r="BY7" s="11"/>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5"/>
@@ -4439,7 +4376,7 @@
       <c r="BX8" s="7"/>
       <c r="BY8" s="12"/>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
@@ -4518,7 +4455,7 @@
       <c r="BX9" s="9"/>
       <c r="BY9" s="11"/>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5"/>
@@ -4597,7 +4534,7 @@
       <c r="BX10" s="7"/>
       <c r="BY10" s="12"/>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
@@ -4676,7 +4613,7 @@
       <c r="BX11" s="9"/>
       <c r="BY11" s="11"/>
     </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:77">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="5"/>
@@ -4755,7 +4692,7 @@
       <c r="BX12" s="7"/>
       <c r="BY12" s="12"/>
     </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:77">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
@@ -4834,7 +4771,7 @@
       <c r="BX13" s="9"/>
       <c r="BY13" s="11"/>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:77">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="5"/>
@@ -4922,9 +4859,5 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D661018-8082-4C74-8BB0-535FAA6BE03A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/DataMashup"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D661018-8082-4C74-8BB0-535FAA6BE03A}"/>
 </file>
</xml_diff>